<commit_message>
11/01/2022 UPDATE: Adding query result processing
</commit_message>
<xml_diff>
--- a/DataWarehouse V2/Results/DataWarehouse Performance Summary.xlsx
+++ b/DataWarehouse V2/Results/DataWarehouse Performance Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOR035\Documents\NetCDFWarehouse\DataWarehouse V2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D4E83A-AFEF-4C38-A044-174824727109}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835F45B6-9C46-4A2B-BF54-1F6768741C84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{493B72DE-E029-4265-817F-6F0C5C250C44}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{493B72DE-E029-4265-817F-6F0C5C250C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="53">
   <si>
     <t>SQ1</t>
   </si>
@@ -194,13 +194,16 @@
   <si>
     <t>Total Ingestion Time (Hours)</t>
   </si>
+  <si>
+    <t>DW7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -288,7 +291,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -360,9 +363,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$6</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -377,16 +380,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$C$2:$C$6</c:f>
+              <c:f>'Elapsed Time'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.2230000000000001</c:v>
                 </c:pt>
@@ -401,6 +410,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>17.844999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4279999999999899</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.486999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -674,9 +689,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>5.3</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -687,12 +699,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$O$2:$O$6</c:f>
+              <c:f>'Total Logical Reads'!$O$2:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>24298351</c:v>
                 </c:pt>
@@ -707,6 +748,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34341782</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25756141</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22836897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -720,9 +767,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>5.2</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -733,12 +777,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$N$2:$N$6</c:f>
+              <c:f>'Total Logical Reads'!$N$2:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>24364718</c:v>
                 </c:pt>
@@ -753,6 +826,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>68668408</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25825625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22908674</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -766,9 +845,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>5.1</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -779,12 +855,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$M$2:$M$6</c:f>
+              <c:f>'Total Logical Reads'!$M$2:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>25102998</c:v>
                 </c:pt>
@@ -799,6 +904,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>68667388</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26615641</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23694445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1038,6 +1149,341 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Ingestion!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total SQL Server Storage (MB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="860000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Ingestion!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Ingestion!$L$2:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>251532.99300000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>251532.93000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>459948.24199999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>317775.24300000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>268105.07</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>268091.44500000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>446347.03099999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4E93-4D5A-81FD-C455388717FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1740046688"/>
+        <c:axId val="1740045024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1740046688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1740045024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1740045024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" b="1"/>
+                  <a:t>SQL SERVER STORAGE (GB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1740046688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -1084,9 +1530,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$6</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -1101,16 +1547,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$D$2:$D$6</c:f>
+              <c:f>'Elapsed Time'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>18.417000000000002</c:v>
                 </c:pt>
@@ -1125,6 +1577,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>163.791</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.365</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.516999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1398,9 +1856,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>3.4</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4"/>
@@ -1411,12 +1866,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$H$2:$H$6</c:f>
+              <c:f>'Elapsed Time'!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>727.00400000000002</c:v>
                 </c:pt>
@@ -1431,6 +1915,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>954.53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>668.84799999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>748.60199999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1444,9 +1934,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>3.3</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -1457,12 +1944,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$G$2:$G$6</c:f>
+              <c:f>'Elapsed Time'!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>717.548</c:v>
                 </c:pt>
@@ -1477,6 +1993,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>748.18799999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>518.82600000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>515.43600000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1490,9 +2012,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>3.2</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -1503,12 +2022,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$F$2:$F$6</c:f>
+              <c:f>'Elapsed Time'!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>386.65699999999998</c:v>
                 </c:pt>
@@ -1523,6 +2071,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>531.80599999999902</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>284.05599999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301.53699999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1536,9 +2090,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:v>3.1</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1551,9 +2102,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$6</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -1568,16 +2119,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$E$2:$E$6</c:f>
+              <c:f>'Elapsed Time'!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>194.952</c:v>
                 </c:pt>
@@ -1592,6 +2149,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>337.45499999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>123.419</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>101.74299999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1865,9 +2428,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>4.4</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4"/>
@@ -1878,12 +2438,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$L$2:$L$6</c:f>
+              <c:f>'Elapsed Time'!$L$2:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>311.67599999999999</c:v>
                 </c:pt>
@@ -1898,6 +2487,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>434.226</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269.589</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>222.78299999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1911,9 +2506,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>4.3</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -1924,12 +2516,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$K$2:$K$6</c:f>
+              <c:f>'Elapsed Time'!$K$2:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>373.87900000000002</c:v>
                 </c:pt>
@@ -1944,6 +2565,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>382.803</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>205.77099999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>224.94399999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1957,9 +2584,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>4.2</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -1970,12 +2594,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$J$2:$J$6</c:f>
+              <c:f>'Elapsed Time'!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>217.13200000000001</c:v>
                 </c:pt>
@@ -1990,6 +2643,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>326.71799999999899</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>136.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>137.37700000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2003,9 +2662,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:v>4.1</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2018,9 +2674,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$6</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -2035,16 +2691,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$I$2:$I$6</c:f>
+              <c:f>'Elapsed Time'!$I$2:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>131.06700000000001</c:v>
                 </c:pt>
@@ -2059,6 +2721,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>266.01400000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86.878</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68.927999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2332,9 +3000,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>5.3</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -2345,12 +3010,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$O$2:$O$6</c:f>
+              <c:f>'Elapsed Time'!$O$2:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>281.79300000000001</c:v>
                 </c:pt>
@@ -2365,6 +3059,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>320.83199999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>147.74799999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>267.077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2378,9 +3078,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>5.2</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -2391,12 +3088,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$N$2:$N$6</c:f>
+              <c:f>'Elapsed Time'!$N$2:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>282.149</c:v>
                 </c:pt>
@@ -2411,6 +3137,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>470.344999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>143.63999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>274.90899999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2424,9 +3156,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>5.1</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2437,12 +3166,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$M$2:$M$6</c:f>
+              <c:f>'Elapsed Time'!$M$2:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>285.52999999999997</c:v>
                 </c:pt>
@@ -2457,6 +3215,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>466.70100000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>148.292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301.09300000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2744,9 +3508,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$6</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -2761,16 +3525,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$C$2:$C$6</c:f>
+              <c:f>'Total Logical Reads'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4043</c:v>
                 </c:pt>
@@ -2785,6 +3555,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3990</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3081,9 +3857,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$6</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -3098,16 +3874,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$D$2:$D$6</c:f>
+              <c:f>'Total Logical Reads'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>808321</c:v>
                 </c:pt>
@@ -3122,6 +3904,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34330562</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>861480</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>861420</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3395,9 +4183,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>3.4</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4"/>
@@ -3408,12 +4193,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$H$2:$H$6</c:f>
+              <c:f>'Total Logical Reads'!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>46445969</c:v>
                 </c:pt>
@@ -3428,6 +4242,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34346780</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34332136</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22833010</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3441,9 +4261,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>3.3</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -3454,12 +4271,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$G$2:$G$6</c:f>
+              <c:f>'Total Logical Reads'!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>34713103</c:v>
                 </c:pt>
@@ -3474,6 +4320,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34343360</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25750783</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25752463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3487,9 +4339,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>3.2</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -3500,12 +4349,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$F$2:$F$6</c:f>
+              <c:f>'Total Logical Reads'!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>38975864</c:v>
                 </c:pt>
@@ -3520,6 +4398,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34338620</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17167323</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17169033</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3533,9 +4417,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:v>3.1</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3548,9 +4429,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$6</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -3565,16 +4446,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$E$2:$E$6</c:f>
+              <c:f>'Total Logical Reads'!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>11126130</c:v>
                 </c:pt>
@@ -3589,6 +4476,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34333544</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8588749</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8588557</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3869,9 +4762,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>4.4</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4"/>
@@ -3882,12 +4772,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$L$2:$L$6</c:f>
+              <c:f>'Total Logical Reads'!$L$2:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>32213766</c:v>
                 </c:pt>
@@ -3902,6 +4821,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34340918</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34331572</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22828205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3915,9 +4840,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>4.3</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -3928,12 +4850,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$K$2:$K$6</c:f>
+              <c:f>'Total Logical Reads'!$K$2:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>24214163</c:v>
                 </c:pt>
@@ -3948,6 +4899,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34338230</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25751623</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25753939</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3961,9 +4918,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>4.2</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -3974,12 +4928,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$J$2:$J$6</c:f>
+              <c:f>'Total Logical Reads'!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>32208894</c:v>
                 </c:pt>
@@ -3994,6 +4977,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34335560</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17168841</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17168583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4007,9 +4996,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:v>4.1</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4022,9 +5008,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$6</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -4039,16 +5025,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$I$2:$I$6</c:f>
+              <c:f>'Total Logical Reads'!$I$2:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>8073346</c:v>
                 </c:pt>
@@ -4063,6 +5055,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34331924</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8588041</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8587621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4343,6 +5341,46 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5680,6 +6718,509 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -10142,6 +11683,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0006F8E-3A87-4688-9E3B-FA402D72B8FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10439,10 +12023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4230BB0A-F4A8-4D4C-8DF2-E07A53F9EEE7}">
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O134"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14592,14 +16176,806 @@
       <c r="N96" s="7"/>
       <c r="O96" s="7"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="B97" t="s">
+        <v>13</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97">
+        <v>18</v>
+      </c>
+      <c r="E97">
+        <v>18</v>
+      </c>
+      <c r="F97">
+        <v>18</v>
+      </c>
+      <c r="G97">
+        <v>18</v>
+      </c>
+      <c r="H97">
+        <v>18</v>
+      </c>
+      <c r="I97">
+        <v>18</v>
+      </c>
+      <c r="J97">
+        <v>18</v>
+      </c>
+      <c r="K97">
+        <v>18</v>
+      </c>
+      <c r="L97">
+        <v>18</v>
+      </c>
+      <c r="M97">
+        <v>45</v>
+      </c>
+      <c r="N97">
+        <v>45</v>
+      </c>
+      <c r="O97">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>14</v>
+      </c>
+      <c r="C98">
+        <v>11</v>
+      </c>
+      <c r="D98">
+        <v>861480</v>
+      </c>
+      <c r="E98">
+        <v>8588749</v>
+      </c>
+      <c r="F98">
+        <v>17167323</v>
+      </c>
+      <c r="G98">
+        <v>25750783</v>
+      </c>
+      <c r="H98">
+        <v>34332136</v>
+      </c>
+      <c r="I98">
+        <v>8588041</v>
+      </c>
+      <c r="J98">
+        <v>17168841</v>
+      </c>
+      <c r="K98">
+        <v>25751623</v>
+      </c>
+      <c r="L98">
+        <v>34331572</v>
+      </c>
+      <c r="M98">
+        <v>26615641</v>
+      </c>
+      <c r="N98">
+        <v>25825625</v>
+      </c>
+      <c r="O98">
+        <v>25756141</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99">
+        <v>4</v>
+      </c>
+      <c r="D99">
+        <v>3</v>
+      </c>
+      <c r="E99">
+        <v>3</v>
+      </c>
+      <c r="F99">
+        <v>3</v>
+      </c>
+      <c r="G99">
+        <v>4</v>
+      </c>
+      <c r="H99">
+        <v>4</v>
+      </c>
+      <c r="I99">
+        <v>3</v>
+      </c>
+      <c r="J99">
+        <v>3</v>
+      </c>
+      <c r="K99">
+        <v>4</v>
+      </c>
+      <c r="L99">
+        <v>4</v>
+      </c>
+      <c r="M99">
+        <v>6</v>
+      </c>
+      <c r="N99">
+        <v>6</v>
+      </c>
+      <c r="O99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>16</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <v>0</v>
+      </c>
+      <c r="N100">
+        <v>0</v>
+      </c>
+      <c r="O100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>17</v>
+      </c>
+      <c r="C101">
+        <v>515</v>
+      </c>
+      <c r="D101">
+        <v>858707</v>
+      </c>
+      <c r="E101">
+        <v>8581445</v>
+      </c>
+      <c r="F101">
+        <v>17158726</v>
+      </c>
+      <c r="G101">
+        <v>25738429</v>
+      </c>
+      <c r="H101">
+        <v>34315768</v>
+      </c>
+      <c r="I101">
+        <v>8581523</v>
+      </c>
+      <c r="J101">
+        <v>17158778</v>
+      </c>
+      <c r="K101">
+        <v>25738465</v>
+      </c>
+      <c r="L101">
+        <v>34315720</v>
+      </c>
+      <c r="M101">
+        <v>26591786</v>
+      </c>
+      <c r="N101">
+        <v>25738451</v>
+      </c>
+      <c r="O101">
+        <v>25740790</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>18</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102">
+        <v>0</v>
+      </c>
+      <c r="N102">
+        <v>0</v>
+      </c>
+      <c r="O102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>19</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103">
+        <v>0</v>
+      </c>
+      <c r="N103">
+        <v>0</v>
+      </c>
+      <c r="O103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>20</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104">
+        <v>0</v>
+      </c>
+      <c r="N104">
+        <v>0</v>
+      </c>
+      <c r="O104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>21</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
+        <v>0</v>
+      </c>
+      <c r="N105">
+        <v>0</v>
+      </c>
+      <c r="O105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>22</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="N106">
+        <v>0</v>
+      </c>
+      <c r="O106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>23</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107">
+        <v>0</v>
+      </c>
+      <c r="N107">
+        <v>0</v>
+      </c>
+      <c r="O107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>24</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108">
+        <v>0</v>
+      </c>
+      <c r="N108">
+        <v>0</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>25</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109">
+        <v>0</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>0</v>
+      </c>
+      <c r="M109">
+        <v>0</v>
+      </c>
+      <c r="N109">
+        <v>0</v>
+      </c>
+      <c r="O109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110">
+        <v>1.4219999999999999</v>
+      </c>
+      <c r="D110">
+        <v>90.702999999999903</v>
+      </c>
+      <c r="E110">
+        <v>758.71600000000001</v>
+      </c>
+      <c r="F110">
+        <v>1667.702</v>
+      </c>
+      <c r="G110">
+        <v>2706.8240000000001</v>
+      </c>
+      <c r="H110">
+        <v>3758.6559999999999</v>
+      </c>
+      <c r="I110">
+        <v>517.45299999999997</v>
+      </c>
+      <c r="J110">
+        <v>1034.4839999999999</v>
+      </c>
+      <c r="K110">
+        <v>1563.0819999999901</v>
+      </c>
+      <c r="L110">
+        <v>2073.6880000000001</v>
+      </c>
+      <c r="M110">
+        <v>1120.9359999999999</v>
+      </c>
+      <c r="N110">
+        <v>1090.672</v>
+      </c>
+      <c r="O110">
+        <v>1106.4059999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>27</v>
+      </c>
+      <c r="C111">
+        <v>1.4279999999999899</v>
+      </c>
+      <c r="D111">
+        <v>12.365</v>
+      </c>
+      <c r="E111">
+        <v>123.419</v>
+      </c>
+      <c r="F111">
+        <v>284.05599999999998</v>
+      </c>
+      <c r="G111">
+        <v>518.82600000000002</v>
+      </c>
+      <c r="H111">
+        <v>668.84799999999996</v>
+      </c>
+      <c r="I111">
+        <v>86.878</v>
+      </c>
+      <c r="J111">
+        <v>136.93</v>
+      </c>
+      <c r="K111">
+        <v>205.77099999999999</v>
+      </c>
+      <c r="L111">
+        <v>269.589</v>
+      </c>
+      <c r="M111">
+        <v>148.292</v>
+      </c>
+      <c r="N111">
+        <v>143.63999999999999</v>
+      </c>
+      <c r="O111">
+        <v>147.74799999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>28</v>
+      </c>
+      <c r="C112">
+        <v>11</v>
+      </c>
+      <c r="D112">
+        <v>861480</v>
+      </c>
+      <c r="E112">
+        <v>8588749</v>
+      </c>
+      <c r="F112">
+        <v>17167323</v>
+      </c>
+      <c r="G112">
+        <v>25750783</v>
+      </c>
+      <c r="H112">
+        <v>34332136</v>
+      </c>
+      <c r="I112">
+        <v>8588041</v>
+      </c>
+      <c r="J112">
+        <v>17168841</v>
+      </c>
+      <c r="K112">
+        <v>25751623</v>
+      </c>
+      <c r="L112">
+        <v>34331572</v>
+      </c>
+      <c r="M112">
+        <v>26615641</v>
+      </c>
+      <c r="N112">
+        <v>25825625</v>
+      </c>
+      <c r="O112">
+        <v>25756141</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>29</v>
+      </c>
+      <c r="C113">
+        <v>515</v>
+      </c>
+      <c r="D113">
+        <v>858707</v>
+      </c>
+      <c r="E113">
+        <v>8581445</v>
+      </c>
+      <c r="F113">
+        <v>17158726</v>
+      </c>
+      <c r="G113">
+        <v>25738429</v>
+      </c>
+      <c r="H113">
+        <v>34315768</v>
+      </c>
+      <c r="I113">
+        <v>8581523</v>
+      </c>
+      <c r="J113">
+        <v>17158778</v>
+      </c>
+      <c r="K113">
+        <v>25738465</v>
+      </c>
+      <c r="L113">
+        <v>34315720</v>
+      </c>
+      <c r="M113">
+        <v>26591786</v>
+      </c>
+      <c r="N113">
+        <v>25738451</v>
+      </c>
+      <c r="O113">
+        <v>25740790</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>30</v>
+      </c>
+      <c r="C114">
+        <v>0.995798319327731</v>
+      </c>
+      <c r="D114">
+        <v>7.3354630004043599</v>
+      </c>
+      <c r="E114">
+        <v>6.1474813440394103</v>
+      </c>
+      <c r="F114">
+        <v>5.8710324724702101</v>
+      </c>
+      <c r="G114">
+        <v>5.2172096232648304</v>
+      </c>
+      <c r="H114">
+        <v>5.6195966796641397</v>
+      </c>
+      <c r="I114">
+        <v>5.9560878473261303</v>
+      </c>
+      <c r="J114">
+        <v>7.5548382385160204</v>
+      </c>
+      <c r="K114">
+        <v>7.5962210418377696</v>
+      </c>
+      <c r="L114">
+        <v>7.69203491240369</v>
+      </c>
+      <c r="M114">
+        <v>7.5589782321365897</v>
+      </c>
+      <c r="N114">
+        <v>7.59309384572542</v>
+      </c>
+      <c r="O114">
+        <v>7.4884668489590398</v>
       </c>
     </row>
     <row r="115" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
-      <c r="B115" s="6"/>
+      <c r="B115" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
@@ -14614,6 +16990,806 @@
       <c r="N115" s="7"/>
       <c r="O115" s="7"/>
     </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B116" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116">
+        <v>18</v>
+      </c>
+      <c r="E116">
+        <v>18</v>
+      </c>
+      <c r="F116">
+        <v>18</v>
+      </c>
+      <c r="G116">
+        <v>18</v>
+      </c>
+      <c r="H116">
+        <v>18</v>
+      </c>
+      <c r="I116">
+        <v>18</v>
+      </c>
+      <c r="J116">
+        <v>18</v>
+      </c>
+      <c r="K116">
+        <v>18</v>
+      </c>
+      <c r="L116">
+        <v>18</v>
+      </c>
+      <c r="M116">
+        <v>45</v>
+      </c>
+      <c r="N116">
+        <v>45</v>
+      </c>
+      <c r="O116">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>14</v>
+      </c>
+      <c r="C117">
+        <v>11</v>
+      </c>
+      <c r="D117">
+        <v>861420</v>
+      </c>
+      <c r="E117">
+        <v>8588557</v>
+      </c>
+      <c r="F117">
+        <v>17169033</v>
+      </c>
+      <c r="G117">
+        <v>25752463</v>
+      </c>
+      <c r="H117">
+        <v>22833010</v>
+      </c>
+      <c r="I117">
+        <v>8587621</v>
+      </c>
+      <c r="J117">
+        <v>17168583</v>
+      </c>
+      <c r="K117">
+        <v>25753939</v>
+      </c>
+      <c r="L117">
+        <v>22828205</v>
+      </c>
+      <c r="M117">
+        <v>23694445</v>
+      </c>
+      <c r="N117">
+        <v>22908674</v>
+      </c>
+      <c r="O117">
+        <v>22836897</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118">
+        <v>6</v>
+      </c>
+      <c r="D118">
+        <v>5</v>
+      </c>
+      <c r="E118">
+        <v>5</v>
+      </c>
+      <c r="F118">
+        <v>5</v>
+      </c>
+      <c r="G118">
+        <v>6</v>
+      </c>
+      <c r="H118">
+        <v>4</v>
+      </c>
+      <c r="I118">
+        <v>5</v>
+      </c>
+      <c r="J118">
+        <v>5</v>
+      </c>
+      <c r="K118">
+        <v>6</v>
+      </c>
+      <c r="L118">
+        <v>4</v>
+      </c>
+      <c r="M118">
+        <v>7</v>
+      </c>
+      <c r="N118">
+        <v>7</v>
+      </c>
+      <c r="O118">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>16</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
+      </c>
+      <c r="M119">
+        <v>0</v>
+      </c>
+      <c r="N119">
+        <v>0</v>
+      </c>
+      <c r="O119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>17</v>
+      </c>
+      <c r="C120">
+        <v>520</v>
+      </c>
+      <c r="D120">
+        <v>858952</v>
+      </c>
+      <c r="E120">
+        <v>8581448</v>
+      </c>
+      <c r="F120">
+        <v>17158780</v>
+      </c>
+      <c r="G120">
+        <v>25738407</v>
+      </c>
+      <c r="H120">
+        <v>22818250</v>
+      </c>
+      <c r="I120">
+        <v>8581463</v>
+      </c>
+      <c r="J120">
+        <v>17158793</v>
+      </c>
+      <c r="K120">
+        <v>25738497</v>
+      </c>
+      <c r="L120">
+        <v>22818238</v>
+      </c>
+      <c r="M120">
+        <v>23675543</v>
+      </c>
+      <c r="N120">
+        <v>22891093</v>
+      </c>
+      <c r="O120">
+        <v>22820599</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>18</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="I121">
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="M121">
+        <v>0</v>
+      </c>
+      <c r="N121">
+        <v>0</v>
+      </c>
+      <c r="O121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>19</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="G122">
+        <v>0</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <v>0</v>
+      </c>
+      <c r="M122">
+        <v>0</v>
+      </c>
+      <c r="N122">
+        <v>0</v>
+      </c>
+      <c r="O122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>20</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+      <c r="H123">
+        <v>0</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123">
+        <v>0</v>
+      </c>
+      <c r="N123">
+        <v>0</v>
+      </c>
+      <c r="O123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>21</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>0</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124">
+        <v>0</v>
+      </c>
+      <c r="N124">
+        <v>0</v>
+      </c>
+      <c r="O124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>22</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>0</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125">
+        <v>0</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
+      </c>
+      <c r="K125">
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+      <c r="M125">
+        <v>0</v>
+      </c>
+      <c r="N125">
+        <v>0</v>
+      </c>
+      <c r="O125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>23</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <v>0</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>0</v>
+      </c>
+      <c r="I126">
+        <v>0</v>
+      </c>
+      <c r="J126">
+        <v>0</v>
+      </c>
+      <c r="K126">
+        <v>0</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
+      </c>
+      <c r="M126">
+        <v>0</v>
+      </c>
+      <c r="N126">
+        <v>0</v>
+      </c>
+      <c r="O126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>24</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <v>0</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127">
+        <v>0</v>
+      </c>
+      <c r="J127">
+        <v>0</v>
+      </c>
+      <c r="K127">
+        <v>0</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+      <c r="M127">
+        <v>0</v>
+      </c>
+      <c r="N127">
+        <v>0</v>
+      </c>
+      <c r="O127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>25</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>0</v>
+      </c>
+      <c r="J128">
+        <v>0</v>
+      </c>
+      <c r="K128">
+        <v>0</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+      <c r="M128">
+        <v>0</v>
+      </c>
+      <c r="N128">
+        <v>0</v>
+      </c>
+      <c r="O128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129">
+        <v>1.9530000000000001</v>
+      </c>
+      <c r="D129">
+        <v>84.092999999999904</v>
+      </c>
+      <c r="E129">
+        <v>708.57999999999902</v>
+      </c>
+      <c r="F129">
+        <v>1780.278</v>
+      </c>
+      <c r="G129">
+        <v>2732.1869999999999</v>
+      </c>
+      <c r="H129">
+        <v>3973.78</v>
+      </c>
+      <c r="I129">
+        <v>523.00099999999998</v>
+      </c>
+      <c r="J129">
+        <v>1048.2919999999999</v>
+      </c>
+      <c r="K129">
+        <v>1584.951</v>
+      </c>
+      <c r="L129">
+        <v>1595.6079999999999</v>
+      </c>
+      <c r="M129">
+        <v>2215.4630000000002</v>
+      </c>
+      <c r="N129">
+        <v>2059.0650000000001</v>
+      </c>
+      <c r="O129">
+        <v>2043.1979999999901</v>
+      </c>
+    </row>
+    <row r="130" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>27</v>
+      </c>
+      <c r="C130">
+        <v>22.486999999999998</v>
+      </c>
+      <c r="D130">
+        <v>12.516999999999999</v>
+      </c>
+      <c r="E130">
+        <v>101.74299999999999</v>
+      </c>
+      <c r="F130">
+        <v>301.53699999999998</v>
+      </c>
+      <c r="G130">
+        <v>515.43600000000004</v>
+      </c>
+      <c r="H130">
+        <v>748.60199999999998</v>
+      </c>
+      <c r="I130">
+        <v>68.927999999999997</v>
+      </c>
+      <c r="J130">
+        <v>137.37700000000001</v>
+      </c>
+      <c r="K130">
+        <v>224.94399999999999</v>
+      </c>
+      <c r="L130">
+        <v>222.78299999999999</v>
+      </c>
+      <c r="M130">
+        <v>301.09300000000002</v>
+      </c>
+      <c r="N130">
+        <v>274.90899999999999</v>
+      </c>
+      <c r="O130">
+        <v>267.077</v>
+      </c>
+    </row>
+    <row r="131" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>28</v>
+      </c>
+      <c r="C131">
+        <v>11</v>
+      </c>
+      <c r="D131">
+        <v>861420</v>
+      </c>
+      <c r="E131">
+        <v>8588557</v>
+      </c>
+      <c r="F131">
+        <v>17169033</v>
+      </c>
+      <c r="G131">
+        <v>25752463</v>
+      </c>
+      <c r="H131">
+        <v>22833010</v>
+      </c>
+      <c r="I131">
+        <v>8587621</v>
+      </c>
+      <c r="J131">
+        <v>17168583</v>
+      </c>
+      <c r="K131">
+        <v>25753939</v>
+      </c>
+      <c r="L131">
+        <v>22828205</v>
+      </c>
+      <c r="M131">
+        <v>23694445</v>
+      </c>
+      <c r="N131">
+        <v>22908674</v>
+      </c>
+      <c r="O131">
+        <v>22836897</v>
+      </c>
+    </row>
+    <row r="132" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>29</v>
+      </c>
+      <c r="C132">
+        <v>520</v>
+      </c>
+      <c r="D132">
+        <v>858952</v>
+      </c>
+      <c r="E132">
+        <v>8581448</v>
+      </c>
+      <c r="F132">
+        <v>17158780</v>
+      </c>
+      <c r="G132">
+        <v>25738407</v>
+      </c>
+      <c r="H132">
+        <v>22818250</v>
+      </c>
+      <c r="I132">
+        <v>8581463</v>
+      </c>
+      <c r="J132">
+        <v>17158793</v>
+      </c>
+      <c r="K132">
+        <v>25738497</v>
+      </c>
+      <c r="L132">
+        <v>22818238</v>
+      </c>
+      <c r="M132">
+        <v>23675543</v>
+      </c>
+      <c r="N132">
+        <v>22891093</v>
+      </c>
+      <c r="O132">
+        <v>22820599</v>
+      </c>
+    </row>
+    <row r="133" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>30</v>
+      </c>
+      <c r="C133">
+        <v>8.6850180104060107E-2</v>
+      </c>
+      <c r="D133">
+        <v>6.7183031077734201</v>
+      </c>
+      <c r="E133">
+        <v>6.9644103279832503</v>
+      </c>
+      <c r="F133">
+        <v>5.90401177964893</v>
+      </c>
+      <c r="G133">
+        <v>5.3007298675296202</v>
+      </c>
+      <c r="H133">
+        <v>5.3082679447823997</v>
+      </c>
+      <c r="I133">
+        <v>7.5876421773444704</v>
+      </c>
+      <c r="J133">
+        <v>7.6307678869097399</v>
+      </c>
+      <c r="K133">
+        <v>7.0459803328828503</v>
+      </c>
+      <c r="L133">
+        <v>7.1621622834776399</v>
+      </c>
+      <c r="M133">
+        <v>7.3580687694499698</v>
+      </c>
+      <c r="N133">
+        <v>7.4899875958953599</v>
+      </c>
+      <c r="O133">
+        <v>7.6502207228626897</v>
+      </c>
+    </row>
+    <row r="134" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14621,10 +17797,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AC055F-86E5-4706-AC7E-BF06FDCFDEC8}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14911,6 +18087,100 @@
         <v>320.83199999999999</v>
       </c>
     </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>1.4279999999999899</v>
+      </c>
+      <c r="D7">
+        <v>12.365</v>
+      </c>
+      <c r="E7">
+        <v>123.419</v>
+      </c>
+      <c r="F7">
+        <v>284.05599999999998</v>
+      </c>
+      <c r="G7">
+        <v>518.82600000000002</v>
+      </c>
+      <c r="H7">
+        <v>668.84799999999996</v>
+      </c>
+      <c r="I7">
+        <v>86.878</v>
+      </c>
+      <c r="J7">
+        <v>136.93</v>
+      </c>
+      <c r="K7">
+        <v>205.77099999999999</v>
+      </c>
+      <c r="L7">
+        <v>269.589</v>
+      </c>
+      <c r="M7">
+        <v>148.292</v>
+      </c>
+      <c r="N7">
+        <v>143.63999999999999</v>
+      </c>
+      <c r="O7">
+        <v>147.74799999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>22.486999999999998</v>
+      </c>
+      <c r="D8">
+        <v>12.516999999999999</v>
+      </c>
+      <c r="E8">
+        <v>101.74299999999999</v>
+      </c>
+      <c r="F8">
+        <v>301.53699999999998</v>
+      </c>
+      <c r="G8">
+        <v>515.43600000000004</v>
+      </c>
+      <c r="H8">
+        <v>748.60199999999998</v>
+      </c>
+      <c r="I8">
+        <v>68.927999999999997</v>
+      </c>
+      <c r="J8">
+        <v>137.37700000000001</v>
+      </c>
+      <c r="K8">
+        <v>224.94399999999999</v>
+      </c>
+      <c r="L8">
+        <v>222.78299999999999</v>
+      </c>
+      <c r="M8">
+        <v>301.09300000000002</v>
+      </c>
+      <c r="N8">
+        <v>274.90899999999999</v>
+      </c>
+      <c r="O8">
+        <v>267.077</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14919,10 +18189,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5260BACE-3E8E-4ABC-9C44-61C910E30632}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O1"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15209,6 +18479,100 @@
         <v>34341782</v>
       </c>
     </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>861480</v>
+      </c>
+      <c r="E7">
+        <v>8588749</v>
+      </c>
+      <c r="F7">
+        <v>17167323</v>
+      </c>
+      <c r="G7">
+        <v>25750783</v>
+      </c>
+      <c r="H7">
+        <v>34332136</v>
+      </c>
+      <c r="I7">
+        <v>8588041</v>
+      </c>
+      <c r="J7">
+        <v>17168841</v>
+      </c>
+      <c r="K7">
+        <v>25751623</v>
+      </c>
+      <c r="L7">
+        <v>34331572</v>
+      </c>
+      <c r="M7">
+        <v>26615641</v>
+      </c>
+      <c r="N7">
+        <v>25825625</v>
+      </c>
+      <c r="O7">
+        <v>25756141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>861420</v>
+      </c>
+      <c r="E8">
+        <v>8588557</v>
+      </c>
+      <c r="F8">
+        <v>17169033</v>
+      </c>
+      <c r="G8">
+        <v>25752463</v>
+      </c>
+      <c r="H8">
+        <v>22833010</v>
+      </c>
+      <c r="I8">
+        <v>8587621</v>
+      </c>
+      <c r="J8">
+        <v>17168583</v>
+      </c>
+      <c r="K8">
+        <v>25753939</v>
+      </c>
+      <c r="L8">
+        <v>22828205</v>
+      </c>
+      <c r="M8">
+        <v>23694445</v>
+      </c>
+      <c r="N8">
+        <v>22908674</v>
+      </c>
+      <c r="O8">
+        <v>22836897</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15217,10 +18581,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D694B81D-3474-4484-97D3-2EC34ECCEEEF}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15402,7 +18766,7 @@
         <v>459948.24199999997</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M3:M6" si="2">(C4+E4)/3600</f>
+        <f t="shared" ref="M4:M6" si="2">(C4+E4)/3600</f>
         <v>29.468611111111112</v>
       </c>
       <c r="N4">
@@ -15504,8 +18868,103 @@
         <v>39.715545790944518</v>
       </c>
     </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7">
+        <v>11794.974</v>
+      </c>
+      <c r="C7" s="12">
+        <v>14400</v>
+      </c>
+      <c r="D7" s="11">
+        <v>152140.85200000001</v>
+      </c>
+      <c r="E7">
+        <v>34184</v>
+      </c>
+      <c r="F7" s="10">
+        <v>266819.32</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1259.336</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>12.718999999999999</v>
+      </c>
+      <c r="K7" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L7" s="10">
+        <f t="shared" ref="L7:L8" si="3">SUM(F7:K7)</f>
+        <v>268091.44500000001</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7:M8" si="4">(C7+E7)/3600</f>
+        <v>13.495555555555555</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ref="N7:N8" si="5">(L7+D7)/B7</f>
+        <v>35.628081672753162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <v>11794.974</v>
+      </c>
+      <c r="C8" s="12">
+        <v>14400</v>
+      </c>
+      <c r="D8" s="11">
+        <v>152140.85200000001</v>
+      </c>
+      <c r="E8">
+        <v>35871</v>
+      </c>
+      <c r="F8" s="10">
+        <v>266819.32</v>
+      </c>
+      <c r="G8" s="10">
+        <v>179514.92199999999</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>12.718999999999999</v>
+      </c>
+      <c r="K8" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="3"/>
+        <v>446347.03099999996</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>13.964166666666667</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="5"/>
+        <v>50.74092431233845</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
12/01/2021: Update with DW7 and DW8
</commit_message>
<xml_diff>
--- a/DataWarehouse V2/Results/DataWarehouse Performance Summary.xlsx
+++ b/DataWarehouse V2/Results/DataWarehouse Performance Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOR035\Documents\NetCDFWarehouse\DataWarehouse V2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835F45B6-9C46-4A2B-BF54-1F6768741C84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA5E3DC-961A-4D3A-ACD8-2A3A442E94EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{493B72DE-E029-4265-817F-6F0C5C250C44}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{493B72DE-E029-4265-817F-6F0C5C250C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="54">
   <si>
     <t>SQ1</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>DW7</t>
+  </si>
+  <si>
+    <t>DW8</t>
   </si>
 </sst>
 </file>
@@ -363,9 +366,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -386,16 +389,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$C$2:$C$8</c:f>
+              <c:f>'Elapsed Time'!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1.2230000000000001</c:v>
                 </c:pt>
@@ -412,10 +418,13 @@
                   <c:v>17.844999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4279999999999899</c:v>
+                  <c:v>0.45899999999999902</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.486999999999998</c:v>
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73199999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -691,162 +700,6 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>DW1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>DW2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>DW3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>DW4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>DW5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>DW6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>DW7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Total Logical Reads'!$O$2:$O$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>24298351</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24298502</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>117796072</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30540222</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34341782</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25756141</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>22836897</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8742-4D0A-AC43-0287E7D1A759}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>DW1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>DW2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>DW3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>DW4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>DW5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>DW6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>DW7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Total Logical Reads'!$N$2:$N$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>24364718</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24364854</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>117795012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30617633</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>68668408</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25825625</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>22908674</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8742-4D0A-AC43-0287E7D1A759}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
@@ -857,9 +710,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -880,43 +733,49 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$M$2:$M$8</c:f>
+              <c:f>'Total Logical Reads'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>25102998</c:v>
+                  <c:v>808321</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25103120</c:v>
+                  <c:v>808321</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117795516</c:v>
+                  <c:v>58892065</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31548156</c:v>
+                  <c:v>1019974</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68667388</c:v>
+                  <c:v>34330562</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26615641</c:v>
+                  <c:v>861480</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23694445</c:v>
+                  <c:v>861606</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>861738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8742-4D0A-AC43-0287E7D1A759}"/>
+              <c16:uniqueId val="{00000000-8ACE-4EAA-9022-1023DA210F5A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1028,7 +887,7 @@
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>Query 5: Logical Reads</a:t>
+                  <a:t>Query 2: Logical Reads</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1508,345 +1367,7 @@
           <c:x val="0.10274277083477398"/>
           <c:y val="7.9494105657169287E-2"/>
           <c:w val="0.84770163442179169"/>
-          <c:h val="0.67697738031357213"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>DW1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>DW2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>DW3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>DW4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>DW5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>DW6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>DW7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Elapsed Time'!$D$2:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>18.417000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.670999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>206.59199999999899</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>163.791</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12.365</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12.516999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0C27-4C85-B5B9-EC13F0402D77}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="103085392"/>
-        <c:axId val="103070832"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="103085392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="103070832"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="103070832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU" b="1">
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>Query 2: Elapsed Time (Seconds)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.27309601924759402"/>
-              <c:y val="0.89521231527009504"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="103085392"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.10274277083477398"/>
-          <c:y val="7.9494105657169287E-2"/>
-          <c:w val="0.84770163442179169"/>
-          <c:h val="0.67697738031357213"/>
+          <c:h val="0.7626916635420572"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1868,9 +1389,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -1891,16 +1412,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$H$2:$H$8</c:f>
+              <c:f>'Elapsed Time'!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>727.00400000000002</c:v>
                 </c:pt>
@@ -1920,7 +1444,10 @@
                   <c:v>668.84799999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>748.60199999999998</c:v>
+                  <c:v>720.96</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>695.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1946,9 +1473,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -1969,16 +1496,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$G$2:$G$8</c:f>
+              <c:f>'Elapsed Time'!$G$2:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>717.548</c:v>
                 </c:pt>
@@ -1998,7 +1528,10 @@
                   <c:v>518.82600000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>515.43600000000004</c:v>
+                  <c:v>475.738</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>491.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2024,9 +1557,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -2047,16 +1580,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$F$2:$F$8</c:f>
+              <c:f>'Elapsed Time'!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>386.65699999999998</c:v>
                 </c:pt>
@@ -2076,7 +1612,10 @@
                   <c:v>284.05599999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>301.53699999999998</c:v>
+                  <c:v>316.58499999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>293.142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2102,9 +1641,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -2125,16 +1664,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$E$2:$E$8</c:f>
+              <c:f>'Elapsed Time'!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>194.952</c:v>
                 </c:pt>
@@ -2154,7 +1696,10 @@
                   <c:v>123.419</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>101.74299999999999</c:v>
+                  <c:v>120.16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>102.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2394,7 +1939,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2418,7 +1963,7 @@
           <c:x val="0.10274277083477398"/>
           <c:y val="7.9494105657169287E-2"/>
           <c:w val="0.84770163442179169"/>
-          <c:h val="0.67697738031357213"/>
+          <c:h val="0.76904086989126363"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2440,9 +1985,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -2463,16 +2008,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$L$2:$L$8</c:f>
+              <c:f>'Elapsed Time'!$L$2:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>311.67599999999999</c:v>
                 </c:pt>
@@ -2492,7 +2040,10 @@
                   <c:v>269.589</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>222.78299999999999</c:v>
+                  <c:v>203.71099999999899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>205.899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2518,9 +2069,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -2541,16 +2092,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$K$2:$K$8</c:f>
+              <c:f>'Elapsed Time'!$K$2:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>373.87900000000002</c:v>
                 </c:pt>
@@ -2570,7 +2124,10 @@
                   <c:v>205.77099999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>224.94399999999999</c:v>
+                  <c:v>212.77699999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>207.31299999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2596,9 +2153,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -2619,16 +2176,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$J$2:$J$8</c:f>
+              <c:f>'Elapsed Time'!$J$2:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>217.13200000000001</c:v>
                 </c:pt>
@@ -2648,7 +2208,10 @@
                   <c:v>136.93</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>137.37700000000001</c:v>
+                  <c:v>136.22499999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>134.387</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2674,9 +2237,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -2697,16 +2260,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$I$2:$I$8</c:f>
+              <c:f>'Elapsed Time'!$I$2:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>131.06700000000001</c:v>
                 </c:pt>
@@ -2726,7 +2292,10 @@
                   <c:v>86.878</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>68.927999999999997</c:v>
+                  <c:v>80.88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73.879000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2966,7 +2535,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2990,7 +2559,7 @@
           <c:x val="0.10274277083477398"/>
           <c:y val="7.9494105657169287E-2"/>
           <c:w val="0.84770163442179169"/>
-          <c:h val="0.67697738031357213"/>
+          <c:h val="0.76904086989126363"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3012,9 +2581,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -3035,16 +2604,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$O$2:$O$8</c:f>
+              <c:f>'Elapsed Time'!$O$2:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>281.79300000000001</c:v>
                 </c:pt>
@@ -3064,7 +2636,10 @@
                   <c:v>147.74799999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>267.077</c:v>
+                  <c:v>301.712999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>302.02600000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3090,9 +2665,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -3113,16 +2688,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$N$2:$N$8</c:f>
+              <c:f>'Elapsed Time'!$N$2:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>282.149</c:v>
                 </c:pt>
@@ -3142,7 +2720,10 @@
                   <c:v>143.63999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>274.90899999999999</c:v>
+                  <c:v>301.03699999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>302.91999999999899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3168,9 +2749,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Elapsed Time'!$A$2:$A$8</c:f>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -3191,16 +2772,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Elapsed Time'!$M$2:$M$8</c:f>
+              <c:f>'Elapsed Time'!$M$2:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>285.52999999999997</c:v>
                 </c:pt>
@@ -3220,7 +2804,10 @@
                   <c:v>148.292</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>301.09300000000002</c:v>
+                  <c:v>338.36899999999901</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>344.77199999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3460,6 +3047,350 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10274277083477398"/>
+          <c:y val="7.9494105657169287E-2"/>
+          <c:w val="0.84770163442179169"/>
+          <c:h val="0.67697738031357213"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Elapsed Time'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Elapsed Time'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>18.417000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.670999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>206.59199999999899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.311999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>163.791</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.365</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.776999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.289</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D34E-46E3-9608-40CFC7FCAD58}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="103085392"/>
+        <c:axId val="103070832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="103085392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103070832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="103070832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" b="1">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Query 2: Elapsed Time (Seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.27309601924759402"/>
+              <c:y val="0.89521231527009504"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103085392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -3508,9 +3439,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -3531,16 +3462,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$C$2:$C$8</c:f>
+              <c:f>'Total Logical Reads'!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>4043</c:v>
                 </c:pt>
@@ -3557,10 +3491,13 @@
                   <c:v>3990</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>3990</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>3990</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3990</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3843,344 +3780,6 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>DW1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>DW2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>DW3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>DW4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>DW5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>DW6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>DW7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Total Logical Reads'!$D$2:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>808321</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>808321</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>58892065</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1019974</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34330562</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>861480</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>861420</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-355B-4708-9FBF-0EDB0B6486AA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="103085392"/>
-        <c:axId val="103070832"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="103085392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="103070832"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="103070832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU" b="1">
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>Query 2: Logical Reads</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.27309601924759402"/>
-              <c:y val="0.89521231527009504"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="103085392"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.10274277083477398"/>
-          <c:y val="7.9494105657169287E-2"/>
-          <c:w val="0.84770163442179169"/>
-          <c:h val="0.67697738031357213"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
           <c:spPr>
@@ -4195,9 +3794,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -4218,16 +3817,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$H$2:$H$8</c:f>
+              <c:f>'Total Logical Reads'!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>46445969</c:v>
                 </c:pt>
@@ -4247,7 +3849,10 @@
                   <c:v>34332136</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22833010</c:v>
+                  <c:v>22832263</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26013373</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4273,9 +3878,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -4296,16 +3901,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$G$2:$G$8</c:f>
+              <c:f>'Total Logical Reads'!$G$2:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>34713103</c:v>
                 </c:pt>
@@ -4325,7 +3933,10 @@
                   <c:v>25750783</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25752463</c:v>
+                  <c:v>25752427</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25750651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4351,9 +3962,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -4374,16 +3985,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$F$2:$F$8</c:f>
+              <c:f>'Total Logical Reads'!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>38975864</c:v>
                 </c:pt>
@@ -4403,7 +4017,10 @@
                   <c:v>17167323</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17169033</c:v>
+                  <c:v>17168847</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17168607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4429,9 +4046,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -4452,16 +4069,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$E$2:$E$8</c:f>
+              <c:f>'Total Logical Reads'!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>11126130</c:v>
                 </c:pt>
@@ -4481,7 +4101,10 @@
                   <c:v>8588749</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8588557</c:v>
+                  <c:v>8588587</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8586439</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4728,7 +4351,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4774,9 +4397,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -4797,16 +4420,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$L$2:$L$8</c:f>
+              <c:f>'Total Logical Reads'!$L$2:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>32213766</c:v>
                 </c:pt>
@@ -4826,7 +4452,10 @@
                   <c:v>34331572</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22828205</c:v>
+                  <c:v>22828618</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26009881</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4852,9 +4481,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -4875,16 +4504,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$K$2:$K$8</c:f>
+              <c:f>'Total Logical Reads'!$K$2:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>24214163</c:v>
                 </c:pt>
@@ -4904,7 +4536,10 @@
                   <c:v>25751623</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25753939</c:v>
+                  <c:v>25751899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25751227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4930,9 +4565,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -4953,16 +4588,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$J$2:$J$8</c:f>
+              <c:f>'Total Logical Reads'!$J$2:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>32208894</c:v>
                 </c:pt>
@@ -4982,7 +4620,10 @@
                   <c:v>17168841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17168583</c:v>
+                  <c:v>17168547</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17168505</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5008,9 +4649,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Total Logical Reads'!$A$2:$A$8</c:f>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -5031,16 +4672,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Logical Reads'!$I$2:$I$8</c:f>
+              <c:f>'Total Logical Reads'!$I$2:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>8073346</c:v>
                 </c:pt>
@@ -5060,7 +4704,10 @@
                   <c:v>8588041</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8587621</c:v>
+                  <c:v>8587243</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8587867</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5180,6 +4827,518 @@
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
                   <a:t>Query 4: Logical Reads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.27309601924759402"/>
+              <c:y val="0.89521231527009504"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103085392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10274277083477398"/>
+          <c:y val="7.9494105657169287E-2"/>
+          <c:w val="0.84770163442179169"/>
+          <c:h val="0.67697738031357213"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Total Logical Reads'!$O$2:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>24298351</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24298502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117796072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30540222</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34341782</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25756141</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22838260</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26020105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8742-4D0A-AC43-0287E7D1A759}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Total Logical Reads'!$N$2:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>24364718</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24364854</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117795012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30617633</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68668408</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25825625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22910200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26091611</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8742-4D0A-AC43-0287E7D1A759}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Total Logical Reads'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>DW1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DW2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DW3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DW4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DW5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DW6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Total Logical Reads'!$M$2:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25102998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25103120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117795516</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31548156</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68667388</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26615641</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23696530</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26878327</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8742-4D0A-AC43-0287E7D1A759}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="103085392"/>
+        <c:axId val="103070832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="103085392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103070832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="103070832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" b="1">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Query 5: Logical Reads</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -11305,7 +11464,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11335,23 +11494,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="17" name="Chart 16">
+        <xdr:cNvPr id="18" name="Chart 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{256C8E48-6001-4734-9BA7-719D2632BE6B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D66BDBF-1706-491C-A940-1A4705107EFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11373,23 +11532,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="18" name="Chart 17">
+        <xdr:cNvPr id="19" name="Chart 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D66BDBF-1706-491C-A940-1A4705107EFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{404E1942-2443-4A1E-AB9F-7CBC913C5905}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11411,23 +11570,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="19" name="Chart 18">
+        <xdr:cNvPr id="20" name="Chart 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{404E1942-2443-4A1E-AB9F-7CBC913C5905}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D53383E4-920A-48B1-B81B-4B699A273B31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11449,23 +11608,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="20" name="Chart 19">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D53383E4-920A-48B1-B81B-4B699A273B31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3B43D6E-405A-430D-A7A9-AC48EF2A9CAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11494,14 +11653,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11530,23 +11689,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AD7C014-FFBB-44F3-BD07-52A166C88653}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF3D3F61-40E7-4DAF-985D-721DF32BB020}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11568,23 +11727,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF3D3F61-40E7-4DAF-985D-721DF32BB020}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECB7FF98-5615-4A55-A736-FBB72049C406}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11606,23 +11765,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>607218</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECB7FF98-5615-4A55-A736-FBB72049C406}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80C590BC-E6C2-426C-A41D-637EF652BA24}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11644,23 +11803,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80C590BC-E6C2-426C-A41D-637EF652BA24}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F00F1C20-7AA1-4F6B-BBA6-E1BF7787C84E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12023,10 +12182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4230BB0A-F4A8-4D4C-8DF2-E07A53F9EEE7}">
-  <dimension ref="A1:O134"/>
+  <dimension ref="A1:O153"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149:O149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16228,7 +16387,7 @@
         <v>14</v>
       </c>
       <c r="C98">
-        <v>11</v>
+        <v>3990</v>
       </c>
       <c r="D98">
         <v>861480</v>
@@ -16272,7 +16431,7 @@
         <v>15</v>
       </c>
       <c r="C99">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D99">
         <v>3</v>
@@ -16360,7 +16519,7 @@
         <v>17</v>
       </c>
       <c r="C101">
-        <v>515</v>
+        <v>3982</v>
       </c>
       <c r="D101">
         <v>858707</v>
@@ -16756,7 +16915,7 @@
         <v>26</v>
       </c>
       <c r="C110">
-        <v>1.4219999999999999</v>
+        <v>0.437</v>
       </c>
       <c r="D110">
         <v>90.702999999999903</v>
@@ -16800,7 +16959,7 @@
         <v>27</v>
       </c>
       <c r="C111">
-        <v>1.4279999999999899</v>
+        <v>0.45899999999999902</v>
       </c>
       <c r="D111">
         <v>12.365</v>
@@ -16844,7 +17003,7 @@
         <v>28</v>
       </c>
       <c r="C112">
-        <v>11</v>
+        <v>3990</v>
       </c>
       <c r="D112">
         <v>861480</v>
@@ -16888,7 +17047,7 @@
         <v>29</v>
       </c>
       <c r="C113">
-        <v>515</v>
+        <v>3982</v>
       </c>
       <c r="D113">
         <v>858707</v>
@@ -16932,7 +17091,7 @@
         <v>30</v>
       </c>
       <c r="C114">
-        <v>0.995798319327731</v>
+        <v>0.95206971677559904</v>
       </c>
       <c r="D114">
         <v>7.3354630004043599</v>
@@ -17042,43 +17201,43 @@
         <v>14</v>
       </c>
       <c r="C117">
-        <v>11</v>
+        <v>3990</v>
       </c>
       <c r="D117">
-        <v>861420</v>
+        <v>861606</v>
       </c>
       <c r="E117">
-        <v>8588557</v>
+        <v>8588587</v>
       </c>
       <c r="F117">
-        <v>17169033</v>
+        <v>17168847</v>
       </c>
       <c r="G117">
-        <v>25752463</v>
+        <v>25752427</v>
       </c>
       <c r="H117">
-        <v>22833010</v>
+        <v>22832263</v>
       </c>
       <c r="I117">
-        <v>8587621</v>
+        <v>8587243</v>
       </c>
       <c r="J117">
-        <v>17168583</v>
+        <v>17168547</v>
       </c>
       <c r="K117">
-        <v>25753939</v>
+        <v>25751899</v>
       </c>
       <c r="L117">
-        <v>22828205</v>
+        <v>22828618</v>
       </c>
       <c r="M117">
-        <v>23694445</v>
+        <v>23696530</v>
       </c>
       <c r="N117">
-        <v>22908674</v>
+        <v>22910200</v>
       </c>
       <c r="O117">
-        <v>22836897</v>
+        <v>22838260</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
@@ -17086,7 +17245,7 @@
         <v>15</v>
       </c>
       <c r="C118">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D118">
         <v>5</v>
@@ -17122,7 +17281,7 @@
         <v>7</v>
       </c>
       <c r="O118">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
@@ -17174,43 +17333,43 @@
         <v>17</v>
       </c>
       <c r="C120">
-        <v>520</v>
+        <v>3982</v>
       </c>
       <c r="D120">
-        <v>858952</v>
+        <v>858947</v>
       </c>
       <c r="E120">
-        <v>8581448</v>
+        <v>8581455</v>
       </c>
       <c r="F120">
-        <v>17158780</v>
+        <v>17158809</v>
       </c>
       <c r="G120">
-        <v>25738407</v>
+        <v>25738465</v>
       </c>
       <c r="H120">
-        <v>22818250</v>
+        <v>22818243</v>
       </c>
       <c r="I120">
-        <v>8581463</v>
+        <v>8581409</v>
       </c>
       <c r="J120">
-        <v>17158793</v>
+        <v>17158790</v>
       </c>
       <c r="K120">
-        <v>25738497</v>
+        <v>25738460</v>
       </c>
       <c r="L120">
-        <v>22818238</v>
+        <v>22818249</v>
       </c>
       <c r="M120">
-        <v>23675543</v>
+        <v>23675537</v>
       </c>
       <c r="N120">
-        <v>22891093</v>
+        <v>22891089</v>
       </c>
       <c r="O120">
-        <v>22820599</v>
+        <v>22820604</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
@@ -17565,230 +17724,1058 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>26</v>
       </c>
       <c r="C129">
-        <v>1.9530000000000001</v>
+        <v>0.51</v>
       </c>
       <c r="D129">
-        <v>84.092999999999904</v>
+        <v>84.074999999999903</v>
       </c>
       <c r="E129">
-        <v>708.57999999999902</v>
+        <v>743.07899999999995</v>
       </c>
       <c r="F129">
-        <v>1780.278</v>
+        <v>1781.0139999999999</v>
       </c>
       <c r="G129">
-        <v>2732.1869999999999</v>
+        <v>2807.123</v>
       </c>
       <c r="H129">
-        <v>3973.78</v>
+        <v>3927.125</v>
       </c>
       <c r="I129">
-        <v>523.00099999999998</v>
+        <v>511.433999999999</v>
       </c>
       <c r="J129">
-        <v>1048.2919999999999</v>
+        <v>1041.55</v>
       </c>
       <c r="K129">
-        <v>1584.951</v>
+        <v>1571.5609999999999</v>
       </c>
       <c r="L129">
-        <v>1595.6079999999999</v>
+        <v>1567.357</v>
       </c>
       <c r="M129">
-        <v>2215.4630000000002</v>
+        <v>2547.9769999999999</v>
       </c>
       <c r="N129">
-        <v>2059.0650000000001</v>
+        <v>2349.2619999999902</v>
       </c>
       <c r="O129">
-        <v>2043.1979999999901</v>
+        <v>2351.39</v>
       </c>
     </row>
-    <row r="130" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>27</v>
       </c>
       <c r="C130">
-        <v>22.486999999999998</v>
+        <v>0.54</v>
       </c>
       <c r="D130">
-        <v>12.516999999999999</v>
+        <v>11.776999999999999</v>
       </c>
       <c r="E130">
-        <v>101.74299999999999</v>
+        <v>120.16</v>
       </c>
       <c r="F130">
-        <v>301.53699999999998</v>
+        <v>316.58499999999998</v>
       </c>
       <c r="G130">
-        <v>515.43600000000004</v>
+        <v>475.738</v>
       </c>
       <c r="H130">
-        <v>748.60199999999998</v>
+        <v>720.96</v>
       </c>
       <c r="I130">
-        <v>68.927999999999997</v>
+        <v>80.88</v>
       </c>
       <c r="J130">
-        <v>137.37700000000001</v>
+        <v>136.22499999999999</v>
       </c>
       <c r="K130">
-        <v>224.94399999999999</v>
+        <v>212.77699999999999</v>
       </c>
       <c r="L130">
-        <v>222.78299999999999</v>
+        <v>203.71099999999899</v>
       </c>
       <c r="M130">
-        <v>301.09300000000002</v>
+        <v>338.36899999999901</v>
       </c>
       <c r="N130">
-        <v>274.90899999999999</v>
+        <v>301.03699999999998</v>
       </c>
       <c r="O130">
-        <v>267.077</v>
+        <v>301.712999999999</v>
       </c>
     </row>
-    <row r="131" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>28</v>
       </c>
       <c r="C131">
-        <v>11</v>
+        <v>3990</v>
       </c>
       <c r="D131">
-        <v>861420</v>
+        <v>861606</v>
       </c>
       <c r="E131">
-        <v>8588557</v>
+        <v>8588587</v>
       </c>
       <c r="F131">
-        <v>17169033</v>
+        <v>17168847</v>
       </c>
       <c r="G131">
-        <v>25752463</v>
+        <v>25752427</v>
       </c>
       <c r="H131">
-        <v>22833010</v>
+        <v>22832263</v>
       </c>
       <c r="I131">
-        <v>8587621</v>
+        <v>8587243</v>
       </c>
       <c r="J131">
-        <v>17168583</v>
+        <v>17168547</v>
       </c>
       <c r="K131">
-        <v>25753939</v>
+        <v>25751899</v>
       </c>
       <c r="L131">
-        <v>22828205</v>
+        <v>22828618</v>
       </c>
       <c r="M131">
-        <v>23694445</v>
+        <v>23696530</v>
       </c>
       <c r="N131">
-        <v>22908674</v>
+        <v>22910200</v>
       </c>
       <c r="O131">
-        <v>22836897</v>
+        <v>22838260</v>
       </c>
     </row>
-    <row r="132" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>29</v>
       </c>
       <c r="C132">
-        <v>520</v>
+        <v>3982</v>
       </c>
       <c r="D132">
-        <v>858952</v>
+        <v>858947</v>
       </c>
       <c r="E132">
-        <v>8581448</v>
+        <v>8581455</v>
       </c>
       <c r="F132">
-        <v>17158780</v>
+        <v>17158809</v>
       </c>
       <c r="G132">
-        <v>25738407</v>
+        <v>25738465</v>
       </c>
       <c r="H132">
-        <v>22818250</v>
+        <v>22818243</v>
       </c>
       <c r="I132">
-        <v>8581463</v>
+        <v>8581409</v>
       </c>
       <c r="J132">
-        <v>17158793</v>
+        <v>17158790</v>
       </c>
       <c r="K132">
-        <v>25738497</v>
+        <v>25738460</v>
       </c>
       <c r="L132">
-        <v>22818238</v>
+        <v>22818249</v>
       </c>
       <c r="M132">
-        <v>23675543</v>
+        <v>23675537</v>
       </c>
       <c r="N132">
-        <v>22891093</v>
+        <v>22891089</v>
       </c>
       <c r="O132">
-        <v>22820599</v>
+        <v>22820604</v>
       </c>
     </row>
-    <row r="133" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>30</v>
       </c>
       <c r="C133">
-        <v>8.6850180104060107E-2</v>
+        <v>0.94444444444444398</v>
       </c>
       <c r="D133">
-        <v>6.7183031077734201</v>
+        <v>7.13891483399847</v>
       </c>
       <c r="E133">
-        <v>6.9644103279832503</v>
+        <v>6.1840795605858796</v>
       </c>
       <c r="F133">
-        <v>5.90401177964893</v>
+        <v>5.6257055767013497</v>
       </c>
       <c r="G133">
-        <v>5.3007298675296202</v>
+        <v>5.90056501687903</v>
       </c>
       <c r="H133">
-        <v>5.3082679447823997</v>
+        <v>5.4470775077674203</v>
       </c>
       <c r="I133">
-        <v>7.5876421773444704</v>
+        <v>6.3233679525222497</v>
       </c>
       <c r="J133">
-        <v>7.6307678869097399</v>
+        <v>7.6458065700128399</v>
       </c>
       <c r="K133">
-        <v>7.0459803328828503</v>
+        <v>7.3859533690201404</v>
       </c>
       <c r="L133">
-        <v>7.1621622834776399</v>
+        <v>7.6940224141062501</v>
       </c>
       <c r="M133">
-        <v>7.3580687694499698</v>
+        <v>7.5301726813035401</v>
       </c>
       <c r="N133">
-        <v>7.4899875958953599</v>
+        <v>7.8038978597315198</v>
       </c>
       <c r="O133">
-        <v>7.6502207228626897</v>
+        <v>7.7934659759440201</v>
       </c>
     </row>
-    <row r="134" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
+    <row r="134" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="6"/>
+      <c r="B134" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="C134" s="7"/>
+      <c r="D134" s="7"/>
+      <c r="E134" s="7"/>
+      <c r="F134" s="7"/>
+      <c r="G134" s="7"/>
+      <c r="H134" s="7"/>
+      <c r="I134" s="7"/>
+      <c r="J134" s="7"/>
+      <c r="K134" s="7"/>
+      <c r="L134" s="7"/>
+      <c r="M134" s="7"/>
+      <c r="N134" s="7"/>
+      <c r="O134" s="7"/>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B135" t="s">
+        <v>13</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <v>18</v>
+      </c>
+      <c r="E135">
+        <v>18</v>
+      </c>
+      <c r="F135">
+        <v>18</v>
+      </c>
+      <c r="G135">
+        <v>18</v>
+      </c>
+      <c r="H135">
+        <v>18</v>
+      </c>
+      <c r="I135">
+        <v>18</v>
+      </c>
+      <c r="J135">
+        <v>18</v>
+      </c>
+      <c r="K135">
+        <v>18</v>
+      </c>
+      <c r="L135">
+        <v>18</v>
+      </c>
+      <c r="M135">
+        <v>45</v>
+      </c>
+      <c r="N135">
+        <v>45</v>
+      </c>
+      <c r="O135">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>14</v>
+      </c>
+      <c r="C136">
+        <v>3990</v>
+      </c>
+      <c r="D136">
+        <v>861738</v>
+      </c>
+      <c r="E136">
+        <v>8586439</v>
+      </c>
+      <c r="F136">
+        <v>17168607</v>
+      </c>
+      <c r="G136">
+        <v>25750651</v>
+      </c>
+      <c r="H136">
+        <v>26013373</v>
+      </c>
+      <c r="I136">
+        <v>8587867</v>
+      </c>
+      <c r="J136">
+        <v>17168505</v>
+      </c>
+      <c r="K136">
+        <v>25751227</v>
+      </c>
+      <c r="L136">
+        <v>26009881</v>
+      </c>
+      <c r="M136">
+        <v>26878327</v>
+      </c>
+      <c r="N136">
+        <v>26091611</v>
+      </c>
+      <c r="O136">
+        <v>26020105</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>15</v>
+      </c>
+      <c r="C137">
+        <v>5</v>
+      </c>
+      <c r="D137">
+        <v>5</v>
+      </c>
+      <c r="E137">
+        <v>5</v>
+      </c>
+      <c r="F137">
+        <v>5</v>
+      </c>
+      <c r="G137">
+        <v>6</v>
+      </c>
+      <c r="H137">
+        <v>5</v>
+      </c>
+      <c r="I137">
+        <v>5</v>
+      </c>
+      <c r="J137">
+        <v>5</v>
+      </c>
+      <c r="K137">
+        <v>6</v>
+      </c>
+      <c r="L137">
+        <v>5</v>
+      </c>
+      <c r="M137">
+        <v>8</v>
+      </c>
+      <c r="N137">
+        <v>8</v>
+      </c>
+      <c r="O137">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>16</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="I138">
+        <v>0</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+      <c r="K138">
+        <v>0</v>
+      </c>
+      <c r="L138">
+        <v>0</v>
+      </c>
+      <c r="M138">
+        <v>0</v>
+      </c>
+      <c r="N138">
+        <v>0</v>
+      </c>
+      <c r="O138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>17</v>
+      </c>
+      <c r="C139">
+        <v>3982</v>
+      </c>
+      <c r="D139">
+        <v>858954</v>
+      </c>
+      <c r="E139">
+        <v>8581397</v>
+      </c>
+      <c r="F139">
+        <v>17158816</v>
+      </c>
+      <c r="G139">
+        <v>25738449</v>
+      </c>
+      <c r="H139">
+        <v>25997008</v>
+      </c>
+      <c r="I139">
+        <v>8581423</v>
+      </c>
+      <c r="J139">
+        <v>17158794</v>
+      </c>
+      <c r="K139">
+        <v>25738410</v>
+      </c>
+      <c r="L139">
+        <v>25997039</v>
+      </c>
+      <c r="M139">
+        <v>26854323</v>
+      </c>
+      <c r="N139">
+        <v>26069859</v>
+      </c>
+      <c r="O139">
+        <v>25999379</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>18</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>0</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+      <c r="K140">
+        <v>0</v>
+      </c>
+      <c r="L140">
+        <v>0</v>
+      </c>
+      <c r="M140">
+        <v>0</v>
+      </c>
+      <c r="N140">
+        <v>0</v>
+      </c>
+      <c r="O140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>19</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+      <c r="K141">
+        <v>0</v>
+      </c>
+      <c r="L141">
+        <v>0</v>
+      </c>
+      <c r="M141">
+        <v>0</v>
+      </c>
+      <c r="N141">
+        <v>0</v>
+      </c>
+      <c r="O141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>20</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+      <c r="I142">
+        <v>0</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+      <c r="K142">
+        <v>0</v>
+      </c>
+      <c r="L142">
+        <v>0</v>
+      </c>
+      <c r="M142">
+        <v>0</v>
+      </c>
+      <c r="N142">
+        <v>0</v>
+      </c>
+      <c r="O142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>21</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+      <c r="H143">
+        <v>0</v>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
+      </c>
+      <c r="K143">
+        <v>0</v>
+      </c>
+      <c r="L143">
+        <v>0</v>
+      </c>
+      <c r="M143">
+        <v>0</v>
+      </c>
+      <c r="N143">
+        <v>0</v>
+      </c>
+      <c r="O143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>22</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <v>0</v>
+      </c>
+      <c r="K144">
+        <v>0</v>
+      </c>
+      <c r="L144">
+        <v>0</v>
+      </c>
+      <c r="M144">
+        <v>0</v>
+      </c>
+      <c r="N144">
+        <v>0</v>
+      </c>
+      <c r="O144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>23</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145">
+        <v>0</v>
+      </c>
+      <c r="L145">
+        <v>0</v>
+      </c>
+      <c r="M145">
+        <v>0</v>
+      </c>
+      <c r="N145">
+        <v>0</v>
+      </c>
+      <c r="O145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>24</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>0</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+      <c r="K146">
+        <v>0</v>
+      </c>
+      <c r="L146">
+        <v>0</v>
+      </c>
+      <c r="M146">
+        <v>0</v>
+      </c>
+      <c r="N146">
+        <v>0</v>
+      </c>
+      <c r="O146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>25</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>0</v>
+      </c>
+      <c r="I147">
+        <v>0</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+      <c r="K147">
+        <v>0</v>
+      </c>
+      <c r="L147">
+        <v>0</v>
+      </c>
+      <c r="M147">
+        <v>0</v>
+      </c>
+      <c r="N147">
+        <v>0</v>
+      </c>
+      <c r="O147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>26</v>
+      </c>
+      <c r="C148">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="D148">
+        <v>87.497999999999905</v>
+      </c>
+      <c r="E148">
+        <v>729.04600000000005</v>
+      </c>
+      <c r="F148">
+        <v>1738.6879999999901</v>
+      </c>
+      <c r="G148">
+        <v>2707.2640000000001</v>
+      </c>
+      <c r="H148">
+        <v>3933.6680000000001</v>
+      </c>
+      <c r="I148">
+        <v>512.29499999999996</v>
+      </c>
+      <c r="J148">
+        <v>1029.4369999999999</v>
+      </c>
+      <c r="K148">
+        <v>1550.84</v>
+      </c>
+      <c r="L148">
+        <v>1584.47</v>
+      </c>
+      <c r="M148">
+        <v>2538.5120000000002</v>
+      </c>
+      <c r="N148">
+        <v>2346.4050000000002</v>
+      </c>
+      <c r="O148">
+        <v>2349.1880000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>27</v>
+      </c>
+      <c r="C149">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="D149">
+        <v>12.289</v>
+      </c>
+      <c r="E149">
+        <v>102.6</v>
+      </c>
+      <c r="F149">
+        <v>293.142</v>
+      </c>
+      <c r="G149">
+        <v>491.96</v>
+      </c>
+      <c r="H149">
+        <v>695.33</v>
+      </c>
+      <c r="I149">
+        <v>73.879000000000005</v>
+      </c>
+      <c r="J149">
+        <v>134.387</v>
+      </c>
+      <c r="K149">
+        <v>207.31299999999999</v>
+      </c>
+      <c r="L149">
+        <v>205.899</v>
+      </c>
+      <c r="M149">
+        <v>344.77199999999999</v>
+      </c>
+      <c r="N149">
+        <v>302.91999999999899</v>
+      </c>
+      <c r="O149">
+        <v>302.02600000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>28</v>
+      </c>
+      <c r="C150">
+        <v>3990</v>
+      </c>
+      <c r="D150">
+        <v>861738</v>
+      </c>
+      <c r="E150">
+        <v>8586439</v>
+      </c>
+      <c r="F150">
+        <v>17168607</v>
+      </c>
+      <c r="G150">
+        <v>25750651</v>
+      </c>
+      <c r="H150">
+        <v>26013373</v>
+      </c>
+      <c r="I150">
+        <v>8587867</v>
+      </c>
+      <c r="J150">
+        <v>17168505</v>
+      </c>
+      <c r="K150">
+        <v>25751227</v>
+      </c>
+      <c r="L150">
+        <v>26009881</v>
+      </c>
+      <c r="M150">
+        <v>26878327</v>
+      </c>
+      <c r="N150">
+        <v>26091611</v>
+      </c>
+      <c r="O150">
+        <v>26020105</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>29</v>
+      </c>
+      <c r="C151">
+        <v>3982</v>
+      </c>
+      <c r="D151">
+        <v>858954</v>
+      </c>
+      <c r="E151">
+        <v>8581397</v>
+      </c>
+      <c r="F151">
+        <v>17158816</v>
+      </c>
+      <c r="G151">
+        <v>25738449</v>
+      </c>
+      <c r="H151">
+        <v>25997008</v>
+      </c>
+      <c r="I151">
+        <v>8581423</v>
+      </c>
+      <c r="J151">
+        <v>17158794</v>
+      </c>
+      <c r="K151">
+        <v>25738410</v>
+      </c>
+      <c r="L151">
+        <v>25997039</v>
+      </c>
+      <c r="M151">
+        <v>26854323</v>
+      </c>
+      <c r="N151">
+        <v>26069859</v>
+      </c>
+      <c r="O151">
+        <v>25999379</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>30</v>
+      </c>
+      <c r="C152">
+        <v>0.96038251366120198</v>
+      </c>
+      <c r="D152">
+        <v>7.1200260395475601</v>
+      </c>
+      <c r="E152">
+        <v>7.1057115009746497</v>
+      </c>
+      <c r="F152">
+        <v>5.9312142238232601</v>
+      </c>
+      <c r="G152">
+        <v>5.50301650540694</v>
+      </c>
+      <c r="H152">
+        <v>5.6572677721369704</v>
+      </c>
+      <c r="I152">
+        <v>6.9342438311292698</v>
+      </c>
+      <c r="J152">
+        <v>7.6602424341640196</v>
+      </c>
+      <c r="K152">
+        <v>7.4806693260914603</v>
+      </c>
+      <c r="L152">
+        <v>7.6953749168281496</v>
+      </c>
+      <c r="M152">
+        <v>7.3628716949172199</v>
+      </c>
+      <c r="N152">
+        <v>7.7459560279941897</v>
+      </c>
+      <c r="O152">
+        <v>7.77809857429492</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="6"/>
+      <c r="B153" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C153" s="7"/>
+      <c r="D153" s="7"/>
+      <c r="E153" s="7"/>
+      <c r="F153" s="7"/>
+      <c r="G153" s="7"/>
+      <c r="H153" s="7"/>
+      <c r="I153" s="7"/>
+      <c r="J153" s="7"/>
+      <c r="K153" s="7"/>
+      <c r="L153" s="7"/>
+      <c r="M153" s="7"/>
+      <c r="N153" s="7"/>
+      <c r="O153" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17797,10 +18784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AC055F-86E5-4706-AC7E-BF06FDCFDEC8}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X44" sqref="X44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18095,7 +19082,7 @@
         <v>27</v>
       </c>
       <c r="C7">
-        <v>1.4279999999999899</v>
+        <v>0.45899999999999902</v>
       </c>
       <c r="D7">
         <v>12.365</v>
@@ -18142,43 +19129,90 @@
         <v>27</v>
       </c>
       <c r="C8">
-        <v>22.486999999999998</v>
+        <v>0.54</v>
       </c>
       <c r="D8">
-        <v>12.516999999999999</v>
+        <v>11.776999999999999</v>
       </c>
       <c r="E8">
-        <v>101.74299999999999</v>
+        <v>120.16</v>
       </c>
       <c r="F8">
-        <v>301.53699999999998</v>
+        <v>316.58499999999998</v>
       </c>
       <c r="G8">
-        <v>515.43600000000004</v>
+        <v>475.738</v>
       </c>
       <c r="H8">
-        <v>748.60199999999998</v>
+        <v>720.96</v>
       </c>
       <c r="I8">
-        <v>68.927999999999997</v>
+        <v>80.88</v>
       </c>
       <c r="J8">
-        <v>137.37700000000001</v>
+        <v>136.22499999999999</v>
       </c>
       <c r="K8">
-        <v>224.94399999999999</v>
+        <v>212.77699999999999</v>
       </c>
       <c r="L8">
-        <v>222.78299999999999</v>
+        <v>203.71099999999899</v>
       </c>
       <c r="M8">
-        <v>301.09300000000002</v>
+        <v>338.36899999999901</v>
       </c>
       <c r="N8">
-        <v>274.90899999999999</v>
+        <v>301.03699999999998</v>
       </c>
       <c r="O8">
-        <v>267.077</v>
+        <v>301.712999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="D9">
+        <v>12.289</v>
+      </c>
+      <c r="E9">
+        <v>102.6</v>
+      </c>
+      <c r="F9">
+        <v>293.142</v>
+      </c>
+      <c r="G9">
+        <v>491.96</v>
+      </c>
+      <c r="H9">
+        <v>695.33</v>
+      </c>
+      <c r="I9">
+        <v>73.879000000000005</v>
+      </c>
+      <c r="J9">
+        <v>134.387</v>
+      </c>
+      <c r="K9">
+        <v>207.31299999999999</v>
+      </c>
+      <c r="L9">
+        <v>205.899</v>
+      </c>
+      <c r="M9">
+        <v>344.77199999999999</v>
+      </c>
+      <c r="N9">
+        <v>302.91999999999899</v>
+      </c>
+      <c r="O9">
+        <v>302.02600000000001</v>
       </c>
     </row>
   </sheetData>
@@ -18189,10 +19223,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5260BACE-3E8E-4ABC-9C44-61C910E30632}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18487,7 +19521,7 @@
         <v>28</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>3990</v>
       </c>
       <c r="D7">
         <v>861480</v>
@@ -18534,43 +19568,90 @@
         <v>28</v>
       </c>
       <c r="C8">
-        <v>11</v>
+        <v>3990</v>
       </c>
       <c r="D8">
-        <v>861420</v>
+        <v>861606</v>
       </c>
       <c r="E8">
-        <v>8588557</v>
+        <v>8588587</v>
       </c>
       <c r="F8">
-        <v>17169033</v>
+        <v>17168847</v>
       </c>
       <c r="G8">
-        <v>25752463</v>
+        <v>25752427</v>
       </c>
       <c r="H8">
-        <v>22833010</v>
+        <v>22832263</v>
       </c>
       <c r="I8">
-        <v>8587621</v>
+        <v>8587243</v>
       </c>
       <c r="J8">
-        <v>17168583</v>
+        <v>17168547</v>
       </c>
       <c r="K8">
-        <v>25753939</v>
+        <v>25751899</v>
       </c>
       <c r="L8">
-        <v>22828205</v>
+        <v>22828618</v>
       </c>
       <c r="M8">
-        <v>23694445</v>
+        <v>23696530</v>
       </c>
       <c r="N8">
-        <v>22908674</v>
+        <v>22910200</v>
       </c>
       <c r="O8">
-        <v>22836897</v>
+        <v>22838260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>3990</v>
+      </c>
+      <c r="D9">
+        <v>861738</v>
+      </c>
+      <c r="E9">
+        <v>8586439</v>
+      </c>
+      <c r="F9">
+        <v>17168607</v>
+      </c>
+      <c r="G9">
+        <v>25750651</v>
+      </c>
+      <c r="H9">
+        <v>26013373</v>
+      </c>
+      <c r="I9">
+        <v>8587867</v>
+      </c>
+      <c r="J9">
+        <v>17168505</v>
+      </c>
+      <c r="K9">
+        <v>25751227</v>
+      </c>
+      <c r="L9">
+        <v>26009881</v>
+      </c>
+      <c r="M9">
+        <v>26878327</v>
+      </c>
+      <c r="N9">
+        <v>26091611</v>
+      </c>
+      <c r="O9">
+        <v>26020105</v>
       </c>
     </row>
   </sheetData>
@@ -18581,10 +19662,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D694B81D-3474-4484-97D3-2EC34ECCEEEF}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18903,15 +19984,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L7" s="10">
-        <f t="shared" ref="L7:L8" si="3">SUM(F7:K7)</f>
+        <f t="shared" ref="L7:L9" si="3">SUM(F7:K7)</f>
         <v>268091.44500000001</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M7:M8" si="4">(C7+E7)/3600</f>
+        <f t="shared" ref="M7:M9" si="4">(C7+E7)/3600</f>
         <v>13.495555555555555</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N8" si="5">(L7+D7)/B7</f>
+        <f t="shared" ref="N7:N9" si="5">(L7+D7)/B7</f>
         <v>35.628081672753162</v>
       </c>
     </row>
@@ -18960,6 +20041,56 @@
       <c r="N8">
         <f t="shared" si="5"/>
         <v>50.74092431233845</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <v>11794.974</v>
+      </c>
+      <c r="C9" s="12">
+        <v>14400</v>
+      </c>
+      <c r="D9" s="11">
+        <v>152140.85200000001</v>
+      </c>
+      <c r="E9">
+        <f>E7+8335</f>
+        <v>42519</v>
+      </c>
+      <c r="F9" s="10">
+        <f>F7+207243.44</f>
+        <v>474062.76</v>
+      </c>
+      <c r="G9" s="11">
+        <f>G7+720.408</f>
+        <v>1979.7440000000001</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>12.718999999999999</v>
+      </c>
+      <c r="K9" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L9" s="10">
+        <f t="shared" si="3"/>
+        <v>476055.29300000001</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>15.810833333333333</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="5"/>
+        <v>53.259646439237592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
14/01/2022 update: first 4 columnstore results
</commit_message>
<xml_diff>
--- a/DataWarehouse V2/Results/DataWarehouse Performance Summary.xlsx
+++ b/DataWarehouse V2/Results/DataWarehouse Performance Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOR035\Documents\NetCDFWarehouse\DataWarehouse V2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA5E3DC-961A-4D3A-ACD8-2A3A442E94EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70670E58-89E5-4DD4-9C90-0E11770D1FE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{493B72DE-E029-4265-817F-6F0C5C250C44}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{493B72DE-E029-4265-817F-6F0C5C250C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="58">
   <si>
     <t>SQ1</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>DW8</t>
+  </si>
+  <si>
+    <t>DW9</t>
+  </si>
+  <si>
+    <t>DW10</t>
+  </si>
+  <si>
+    <t>DW11</t>
+  </si>
+  <si>
+    <t>DW12</t>
   </si>
 </sst>
 </file>
@@ -1057,9 +1069,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Ingestion!$A$2:$A$8</c:f>
+              <c:f>Ingestion!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>DW1</c:v>
                 </c:pt>
@@ -1080,16 +1092,28 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>DW7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DW8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>DW9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DW10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>DW11</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ingestion!$L$2:$L$8</c:f>
+              <c:f>Ingestion!$L$2:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>251532.99300000002</c:v>
                 </c:pt>
@@ -1110,6 +1134,15 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>446347.03099999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>476055.29300000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59610.954000000012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59610.954000000012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12184,7 +12217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4230BB0A-F4A8-4D4C-8DF2-E07A53F9EEE7}">
   <dimension ref="A1:O153"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B149" sqref="B149:O149"/>
     </sheetView>
   </sheetViews>
@@ -18787,7 +18820,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X44" sqref="X44"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19225,8 +19258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5260BACE-3E8E-4ABC-9C44-61C910E30632}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19662,10 +19695,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D694B81D-3474-4484-97D3-2EC34ECCEEEF}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19796,7 +19829,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L3" s="10">
-        <f t="shared" ref="L3:L6" si="0">SUM(F3:K3)</f>
+        <f t="shared" ref="L3:L5" si="0">SUM(F3:K3)</f>
         <v>251532.93000000002</v>
       </c>
       <c r="M3">
@@ -19847,7 +19880,7 @@
         <v>459948.24199999997</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M6" si="2">(C4+E4)/3600</f>
+        <f t="shared" ref="M4:M5" si="2">(C4+E4)/3600</f>
         <v>29.468611111111112</v>
       </c>
       <c r="N4">
@@ -19937,11 +19970,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L6" s="10">
-        <f t="shared" si="0"/>
+        <f>SUM(F6:K6)</f>
         <v>268105.07</v>
       </c>
       <c r="M6">
-        <f t="shared" si="2"/>
+        <f>(C6+E6)/3600</f>
         <v>25.883333333333333</v>
       </c>
       <c r="N6">
@@ -20092,6 +20125,165 @@
         <f t="shared" si="5"/>
         <v>53.259646439237592</v>
       </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
+        <v>11794.974</v>
+      </c>
+      <c r="C10" s="12">
+        <v>14400</v>
+      </c>
+      <c r="D10" s="11">
+        <v>152140.85200000001</v>
+      </c>
+      <c r="E10">
+        <v>10320</v>
+      </c>
+      <c r="F10" s="10">
+        <v>59608.641000000003</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I10">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J10">
+        <v>2.2810000000000001</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0</v>
+      </c>
+      <c r="L10" s="10">
+        <f t="shared" ref="L10:L11" si="6">SUM(F10:K10)</f>
+        <v>59610.954000000012</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10:M12" si="7">(C10+E10)/3600</f>
+        <v>6.8666666666666663</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ref="N10:N12" si="8">(L10+D10)/B10</f>
+        <v>17.952714944517897</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>11794.974</v>
+      </c>
+      <c r="C11" s="12">
+        <v>14400</v>
+      </c>
+      <c r="D11" s="11">
+        <v>152140.85200000001</v>
+      </c>
+      <c r="E11">
+        <v>10320</v>
+      </c>
+      <c r="F11" s="10">
+        <v>59608.641000000003</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I11">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J11">
+        <v>2.2810000000000001</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="10">
+        <f>SUM(F11:K11)</f>
+        <v>59610.954000000012</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="7"/>
+        <v>6.8666666666666663</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="8"/>
+        <v>17.952714944517897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>11794.974</v>
+      </c>
+      <c r="C12" s="12">
+        <v>68400</v>
+      </c>
+      <c r="D12" s="11">
+        <v>252155.609</v>
+      </c>
+      <c r="E12" s="10">
+        <v>24015</v>
+      </c>
+      <c r="F12" s="10">
+        <v>49121.366999999998</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+      <c r="L12" s="10">
+        <f>SUM(F12:K12)</f>
+        <v>49121.366999999998</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="7"/>
+        <v>25.670833333333334</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="8"/>
+        <v>25.542826631071847</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>11794.974</v>
+      </c>
+      <c r="C13" s="12">
+        <v>14400</v>
+      </c>
+      <c r="D13" s="11">
+        <v>152140.85200000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="12"/>
+      <c r="D14" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>